<commit_message>
Update Rizka - 1 Juni 2020 PreProd
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\ACCPartner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC94FDA-94EB-401A-9D8C-59062F299F1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C38B2D7-8B93-495A-9A90-84A3AC7D1C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{23D465F3-B56E-40A1-9EB0-7556D0AF945C}"/>
   </bookViews>
   <sheets>
     <sheet name="Daftar - KACAB dan ADMIN HEAD" sheetId="1" r:id="rId1"/>
+    <sheet name="Daftar - SUPERVISOR &amp; SALESMAN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="81">
   <si>
     <t>referralCode</t>
   </si>
@@ -62,9 +63,6 @@
     <t>info</t>
   </si>
   <si>
-    <t>1S2EIP</t>
-  </si>
-  <si>
     <t>batal</t>
   </si>
   <si>
@@ -246,6 +244,39 @@
   </si>
   <si>
     <t>Rizqo</t>
+  </si>
+  <si>
+    <t>SALESMAN</t>
+  </si>
+  <si>
+    <t>SUPERVISOR</t>
+  </si>
+  <si>
+    <t>812332659854</t>
+  </si>
+  <si>
+    <t>812332659855</t>
+  </si>
+  <si>
+    <t>xyzxyz20@gmail.com</t>
+  </si>
+  <si>
+    <t>xyzxyz21@gmail.com</t>
+  </si>
+  <si>
+    <t>rizkajuliant36</t>
+  </si>
+  <si>
+    <t>rizkajuliant37</t>
+  </si>
+  <si>
+    <t>Rizqy</t>
+  </si>
+  <si>
+    <t>Rizqu</t>
+  </si>
+  <si>
+    <t>74DIGC</t>
   </si>
 </sst>
 </file>
@@ -880,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AF8566-A96D-4791-ACB3-A010E8C73DF7}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,46 +963,46 @@
         <v>7</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="N1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>8</v>
@@ -998,16 +1029,16 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1033,21 +1064,21 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1068,40 +1099,40 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1115,42 +1146,42 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1164,40 +1195,40 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1211,42 +1242,42 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1260,42 +1291,42 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1309,42 +1340,42 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="8">
         <v>12345678</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1358,40 +1389,40 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1405,42 +1436,42 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1454,42 +1485,42 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1503,40 +1534,40 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1550,42 +1581,42 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="8">
         <v>812</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1599,42 +1630,42 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="8">
         <v>31649457757</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1648,40 +1679,40 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1695,42 +1726,42 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1744,42 +1775,42 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1793,42 +1824,42 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="8">
         <v>1234567</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1842,39 +1873,39 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="1"/>
@@ -1889,42 +1920,42 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -1938,42 +1969,42 @@
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V22" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W22" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -1987,42 +2018,42 @@
       <c r="R23" s="14"/>
       <c r="S23" s="14"/>
       <c r="T23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V23" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W23" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2048,42 +2079,42 @@
         <v>1</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W24" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -2109,40 +2140,40 @@
         <v>5</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W25" s="20"/>
     </row>
     <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
@@ -2168,13 +2199,13 @@
         <v>5</v>
       </c>
       <c r="T26" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V26" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W26" s="24"/>
     </row>
@@ -2183,4 +2214,1311 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549D4DF4-2F8E-45DC-A831-0CB39BA8C572}">
+  <dimension ref="A1:W26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A1:A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>123</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8">
+        <v>12345678</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="8">
+        <v>812</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="8">
+        <v>31649457757</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1234567</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W22" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="U23" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="W23" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1</v>
+      </c>
+      <c r="P24" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1">
+        <v>1</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W24" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4">
+        <v>3</v>
+      </c>
+      <c r="O25" s="4">
+        <v>5</v>
+      </c>
+      <c r="P25" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>1</v>
+      </c>
+      <c r="R25" s="4">
+        <v>9</v>
+      </c>
+      <c r="S25" s="4">
+        <v>5</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="W25" s="20"/>
+    </row>
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22">
+        <v>3</v>
+      </c>
+      <c r="O26" s="22">
+        <v>5</v>
+      </c>
+      <c r="P26" s="22">
+        <v>6</v>
+      </c>
+      <c r="Q26" s="22">
+        <v>1</v>
+      </c>
+      <c r="R26" s="22">
+        <v>9</v>
+      </c>
+      <c r="S26" s="22">
+        <v>5</v>
+      </c>
+      <c r="T26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="W26" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Rizka - 3 Juli 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\ACCPartner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C38B2D7-8B93-495A-9A90-84A3AC7D1C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4B42C3-E4A7-477D-A2FB-8F8B98E7E01F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{23D465F3-B56E-40A1-9EB0-7556D0AF945C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="3" xr2:uid="{23D465F3-B56E-40A1-9EB0-7556D0AF945C}"/>
   </bookViews>
   <sheets>
     <sheet name="Daftar - KACAB dan ADMIN HEAD" sheetId="1" r:id="rId1"/>
-    <sheet name="Daftar - SUPERVISOR &amp; SALESMAN" sheetId="2" r:id="rId2"/>
+    <sheet name="Login - Logout" sheetId="3" r:id="rId2"/>
+    <sheet name="Daftar - SUPERVISOR &amp; SALESMAN" sheetId="2" r:id="rId3"/>
+    <sheet name="Lupa Password" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="120">
   <si>
     <t>referralCode</t>
   </si>
@@ -277,6 +279,123 @@
   </si>
   <si>
     <t>74DIGC</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>A123AAA</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>infoCase</t>
+  </si>
+  <si>
+    <t>infoCondition</t>
+  </si>
+  <si>
+    <t>allEmpty</t>
+  </si>
+  <si>
+    <t>passEmpty</t>
+  </si>
+  <si>
+    <t>unameEmpty</t>
+  </si>
+  <si>
+    <t>accNotRegistered</t>
+  </si>
+  <si>
+    <t>r38</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>notValid</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>rizkawiwi10</t>
+  </si>
+  <si>
+    <t>unameOrPassIncorrect</t>
+  </si>
+  <si>
+    <t>lupaUsername</t>
+  </si>
+  <si>
+    <t>lupaPassword</t>
+  </si>
+  <si>
+    <t>kataSandiBaru</t>
+  </si>
+  <si>
+    <t>verifKataSandiBaru</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>infoHelp</t>
+  </si>
+  <si>
+    <t>rizkariz20@gmail.com</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Hshs</t>
+  </si>
+  <si>
+    <t>usernameInvalid</t>
+  </si>
+  <si>
+    <t>passAlfanumerik</t>
+  </si>
+  <si>
+    <t>conPassTidakSama</t>
+  </si>
+  <si>
+    <t>fieldKeduanyaKosong</t>
+  </si>
+  <si>
+    <t>A123444</t>
+  </si>
+  <si>
+    <t>rizkajuliant23</t>
+  </si>
+  <si>
+    <t>rizkajuliant24</t>
+  </si>
+  <si>
+    <t>rizkajuliant25</t>
+  </si>
+  <si>
+    <t>rizkajuliant26</t>
+  </si>
+  <si>
+    <t>passKurang</t>
+  </si>
+  <si>
+    <t>conPassKurang</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>verifVia</t>
   </si>
 </sst>
 </file>
@@ -308,7 +427,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +452,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -514,11 +651,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,6 +814,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -911,7 +1195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AF8566-A96D-4791-ACB3-A010E8C73DF7}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -919,7 +1203,7 @@
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -2217,11 +2501,192 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B32AC1-EE4D-49B9-9EA7-0DC4BF72E192}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549D4DF4-2F8E-45DC-A831-0CB39BA8C572}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A1:A26"/>
+    <sheetView topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26:S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3521,4 +3986,590 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36212998-F113-493F-94B5-99F6AB3DDB3F}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="36"/>
+      <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="36"/>
+      <c r="B8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>9</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1234567</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="36"/>
+      <c r="B10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>9</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="37"/>
+      <c r="B11" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="34">
+        <v>3</v>
+      </c>
+      <c r="E11" s="34">
+        <v>5</v>
+      </c>
+      <c r="F11" s="34">
+        <v>6</v>
+      </c>
+      <c r="G11" s="34">
+        <v>1</v>
+      </c>
+      <c r="H11" s="34">
+        <v>9</v>
+      </c>
+      <c r="I11" s="34">
+        <v>5</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="35"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N15" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="34">
+        <v>3</v>
+      </c>
+      <c r="E16" s="34">
+        <v>5</v>
+      </c>
+      <c r="F16" s="34">
+        <v>6</v>
+      </c>
+      <c r="G16" s="34">
+        <v>1</v>
+      </c>
+      <c r="H16" s="34">
+        <v>9</v>
+      </c>
+      <c r="I16" s="34">
+        <v>5</v>
+      </c>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="N16" s="35"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Rizka - 4 Juli 2020
</commit_message>
<xml_diff>
--- a/Data Binding_Rizka.xlsx
+++ b/Data Binding_Rizka.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\WORKS (TUGAS)\ACCPartner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06101CF9-EB59-41DD-B1B3-5C7DB35AC706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3071A02F-3E65-48F1-B8A0-C76FA54FE6E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="3" xr2:uid="{23D465F3-B56E-40A1-9EB0-7556D0AF945C}"/>
+    <workbookView xWindow="3675" yWindow="15" windowWidth="13410" windowHeight="11055" firstSheet="4" activeTab="5" xr2:uid="{23D465F3-B56E-40A1-9EB0-7556D0AF945C}"/>
   </bookViews>
   <sheets>
     <sheet name="Daftar - KACAB dan ADMIN HEAD" sheetId="1" r:id="rId1"/>
     <sheet name="Login - Logout" sheetId="3" r:id="rId2"/>
     <sheet name="Daftar - SUPERVISOR &amp; SALESMAN" sheetId="2" r:id="rId3"/>
     <sheet name="Lupa Password" sheetId="4" r:id="rId4"/>
+    <sheet name="Edit Foto Profil" sheetId="5" r:id="rId5"/>
+    <sheet name="Info dan Berita ACC" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="125">
   <si>
     <t>referralCode</t>
   </si>
@@ -387,6 +389,30 @@
   </si>
   <si>
     <t>otpKosong</t>
+  </si>
+  <si>
+    <t>photoName</t>
+  </si>
+  <si>
+    <t>camera</t>
+  </si>
+  <si>
+    <t>retake</t>
+  </si>
+  <si>
+    <t>infoCamera</t>
+  </si>
+  <si>
+    <t>gallery</t>
+  </si>
+  <si>
+    <t>japanese</t>
+  </si>
+  <si>
+    <t>namaInfo</t>
+  </si>
+  <si>
+    <t>Hai</t>
   </si>
 </sst>
 </file>
@@ -3983,7 +4009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36212998-F113-493F-94B5-99F6AB3DDB3F}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -4615,4 +4641,137 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A66C638-9585-4542-81B5-98A761C95059}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{605AFCE4-0D0F-4A71-8444-A69BC52981A1}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>